<commit_message>
update file phân chia coong việc
</commit_message>
<xml_diff>
--- a/bc54-final project-vudai.xlsx
+++ b/bc54-final project-vudai.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
   <si>
     <t>Tasks Name</t>
   </si>
@@ -90,6 +90,12 @@
   </si>
   <si>
     <t>đai</t>
+  </si>
+  <si>
+    <t>adminpage</t>
+  </si>
+  <si>
+    <t>thanh</t>
   </si>
 </sst>
 </file>
@@ -589,7 +595,7 @@
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -805,7 +811,28 @@
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
     </row>
-    <row r="10" spans="1:10" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:10" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="2">
+        <v>45289</v>
+      </c>
+      <c r="C10" s="2">
+        <v>45326</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+    </row>
     <row r="11" spans="1:10" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:10" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:10" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>